<commit_message>
Matte er gøy og kult og alle de kule folkene gjør matte hele tida
</commit_message>
<xml_diff>
--- a/Matte3/ULTIEMATEMATH/Matte matriser.xlsx
+++ b/Matte3/ULTIEMATEMATH/Matte matriser.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adama\OneDrive\Dokumenter\GitHub\SkoleStuff\Matte3\ULTIEMATEMATH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C33AD9-4227-4BAB-A08E-ED551F419381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E87F5A4-DBB8-49CD-8B56-7FCE8F82FAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1EFBE4A-FEBF-4BB1-BE4B-BE64A4BEC692}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDCFE0B-9B23-4A68-8D19-CA1C23218893}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E126" sqref="E125:E126"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="R87" sqref="R87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1486,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L97" t="s">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="R97" t="s">
+        <v>3</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -1494,23 +1517,105 @@
         <f t="array" ref="B98:B101">MMULT(_xlfn.ANCHORARRAY(B92),H86:H89)</f>
         <v>8.9285714285714288E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M98">
+        <v>1</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
+      <c r="O98">
+        <v>1</v>
+      </c>
+      <c r="P98">
+        <v>1</v>
+      </c>
+      <c r="S98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B99" s="4">
         <v>-2.125</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>1</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B100" s="4">
         <v>3.0357142857142856</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M100">
+        <v>3</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+      <c r="O100">
+        <v>1</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B101" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L103" t="e" cm="1">
+        <f t="array" ref="L103">MINVERSE(M97:P100)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M103" t="e" cm="1">
+        <f t="array" ref="M103">MINVERSE(N97:Q100)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N103" t="e" cm="1">
+        <f t="array" ref="N103">MINVERSE(O97:R100)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O103" t="e" cm="1">
+        <f t="array" ref="O103">MINVERSE(P97:S100)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L104" t="e" cm="1">
+        <f t="array" ref="L104">MINVERSE(M98:P101)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M104" t="e" cm="1">
+        <f t="array" ref="M104">MINVERSE(N98:Q101)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N104" t="e" cm="1">
+        <f t="array" ref="N104">MINVERSE(O98:R101)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O104" t="e" cm="1">
+        <f t="array" ref="O104">MINVERSE(P98:S101)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -1523,8 +1628,24 @@
       <c r="D105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L105" t="e" cm="1">
+        <f t="array" ref="L105">MINVERSE(M99:P102)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M105" t="e" cm="1">
+        <f t="array" ref="M105">MINVERSE(N99:Q102)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N105" t="e" cm="1">
+        <f t="array" ref="N105">MINVERSE(O99:R102)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O105" t="e" cm="1">
+        <f t="array" ref="O105">MINVERSE(P99:S102)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1</v>
       </c>
@@ -1537,8 +1658,24 @@
       <c r="D106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L106" t="e" cm="1">
+        <f t="array" ref="L106">MINVERSE(M100:P103)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M106" t="e" cm="1">
+        <f t="array" ref="M106">MINVERSE(N100:Q103)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N106" t="e" cm="1">
+        <f t="array" ref="N106">MINVERSE(O100:R103)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O106" t="e" cm="1">
+        <f t="array" ref="O106">MINVERSE(P100:S103)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -1552,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>3</v>
       </c>
@@ -1566,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
         <v>11</v>
       </c>
@@ -1580,7 +1717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" cm="1">
         <f t="array" ref="A112:D115">MINVERSE(A105:D108)</f>
         <v>1.9999999999999998</v>
@@ -1755,6 +1892,95 @@
       </c>
       <c r="H121">
         <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>3</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134" t="e" cm="1">
+        <f t="array" ref="B134">MINVERSE(B128:E131)</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>